<commit_message>
Plot history rate with standard deviation
</commit_message>
<xml_diff>
--- a/历史出率.xlsx
+++ b/历史出率.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Vtuber\Tools\GachaStatistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FC0ECD2-E03B-4E4B-9C00-D94EFA23D895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FB73F4-77AE-41B7-85C9-5B0E05CD1E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,27 @@
     <sheet name="方舟" sheetId="1" r:id="rId1"/>
     <sheet name="原神" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>日期</t>
   </si>
@@ -68,6 +78,12 @@
   </si>
   <si>
     <t>角色</t>
+  </si>
+  <si>
+    <t>标准差（上）</t>
+  </si>
+  <si>
+    <t>标准差（下）</t>
   </si>
 </sst>
 </file>
@@ -121,6 +137,1182 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="zh-CN"/>
+              <a:t>原神历史出率</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>原神!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>六星出率</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>原神!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>神里绫华</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>雷神</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>心海</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>胡桃</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>申鹤</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>钟离/甘雨</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>八重神子</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>原神!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.65</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.04</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.83</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A8D5-4E98-9001-C2A6FA8F266A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>原神!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>up出率</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>原神!$E$2:$E$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>1.44</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.23</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.93</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.19</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.42</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.21</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.03</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>原神!$F$2:$F$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>1.05</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>1.23</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.93</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.06</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.42</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.21</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.03</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>原神!$B$2:$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>神里绫华</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>雷神</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>心海</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>胡桃</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>申鹤</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>钟离/甘雨</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>八重神子</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>原神!$D$2:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.07</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.39</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.08</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.47</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.43</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.32</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A8D5-4E98-9001-C2A6FA8F266A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="988690144"/>
+        <c:axId val="988686816"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="988690144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="988686816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="988686816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="988690144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A516CD4-0756-4119-9121-FA261BE03381}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -413,7 +1605,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F2CCC9-7810-43B3-B79E-716FDC852CE6}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -422,7 +1614,7 @@
     <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,10 +1628,13 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>44398</v>
       </c>
@@ -455,8 +1650,12 @@
       <c r="E2">
         <v>1.44</v>
       </c>
+      <c r="F2">
+        <f>MIN(D2 - 0.02,E2)</f>
+        <v>1.05</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>44440</v>
       </c>
@@ -472,8 +1671,12 @@
       <c r="E3">
         <v>1.23</v>
       </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F8" si="0">MIN(D3 - 0.02,E3)</f>
+        <v>1.23</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>44460</v>
       </c>
@@ -489,8 +1692,12 @@
       <c r="E4">
         <v>0.93</v>
       </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.93</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>44502</v>
       </c>
@@ -506,8 +1713,12 @@
       <c r="E5">
         <v>1.19</v>
       </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1.06</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>44566</v>
       </c>
@@ -523,8 +1734,12 @@
       <c r="E6">
         <v>1.42</v>
       </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1.42</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1">
         <v>44586</v>
       </c>
@@ -540,8 +1755,12 @@
       <c r="E7">
         <v>1.21</v>
       </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1.21</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1">
         <v>44608</v>
       </c>
@@ -555,10 +1774,15 @@
         <v>1.32</v>
       </c>
       <c r="E8">
+        <v>1.03</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
         <v>1.03</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update for 3/15 Fiammetta
</commit_message>
<xml_diff>
--- a/历史出率.xlsx
+++ b/历史出率.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Vtuber\Tools\GachaStatistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EEFA799-5347-4712-B631-F92FAD679ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC24F04-098D-4224-B902-BD018B8DB24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="16080" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="方舟" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>日期</t>
   </si>
@@ -85,6 +85,30 @@
   <si>
     <t>五星出率</t>
   </si>
+  <si>
+    <t>帕拉斯</t>
+  </si>
+  <si>
+    <t>陈和水月</t>
+  </si>
+  <si>
+    <t>琴柳</t>
+  </si>
+  <si>
+    <t>远牙</t>
+  </si>
+  <si>
+    <t>临光焰尾</t>
+  </si>
+  <si>
+    <t>灵知</t>
+  </si>
+  <si>
+    <t>令和老鲤</t>
+  </si>
+  <si>
+    <t>澄闪</t>
+  </si>
 </sst>
 </file>
 
@@ -119,9 +143,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -140,6 +165,514 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="zh-CN"/>
+              <a:t>方舟历史出率</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>方舟!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>六星出率</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>方舟!$B$2:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>帕拉斯</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>陈和水月</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>琴柳</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>远牙</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>临光焰尾</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>灵知</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>令和老鲤</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>澄闪</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>方舟!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>3.2199999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4799999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6900000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.6499999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.3099999999999997E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DD1F-4B3E-B702-B739F56A584F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>方舟!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>up出率</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>方舟!$B$2:$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>帕拉斯</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>陈和水月</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>琴柳</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>远牙</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>临光焰尾</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>灵知</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>令和老鲤</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>澄闪</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>方舟!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.3300000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6400000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7600000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.44E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.78E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.89E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DD1F-4B3E-B702-B739F56A584F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="969251376"/>
+        <c:axId val="1420328864"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="969251376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1420328864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1420328864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="5.000000000000001E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="969251376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -290,31 +823,31 @@
             <c:numRef>
               <c:f>原神!$C$2:$C$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.76</c:v>
+                  <c:v>1.7600000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6</c:v>
+                  <c:v>1.6E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.65</c:v>
+                  <c:v>1.6500000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.04</c:v>
+                  <c:v>2.0400000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.83</c:v>
+                  <c:v>1.83E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.79</c:v>
+                  <c:v>1.7899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.49</c:v>
+                  <c:v>1.49E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -365,88 +898,6 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>原神!$E$2:$E$9</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="8"/>
-                  <c:pt idx="0">
-                    <c:v>1.44</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>1.23</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.93</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.19</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.42</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>1.21</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>1.03</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>1.07</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>原神!$F$2:$F$9</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="8"/>
-                  <c:pt idx="0">
-                    <c:v>1.05</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>1.23</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.93</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.06</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.42</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>1.21</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>1.03</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0.76</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="25400">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>原神!$B$2:$B$9</c:f>
@@ -483,31 +934,31 @@
             <c:numRef>
               <c:f>原神!$D$2:$D$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.07</c:v>
+                  <c:v>1.0699999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.39</c:v>
+                  <c:v>1.3899999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1499999999999999</c:v>
+                  <c:v>1.15E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.08</c:v>
+                  <c:v>1.0800000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.47</c:v>
+                  <c:v>1.47E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.43</c:v>
+                  <c:v>1.43E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.32</c:v>
+                  <c:v>1.32E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.78</c:v>
+                  <c:v>7.7999999999999996E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -601,10 +1052,11 @@
         <c:axId val="988686816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="5.000000000000001E-2"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -768,7 +1220,568 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1294,15 +2307,56 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>85724</xdr:rowOff>
+      <xdr:rowOff>9523</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDCC13C0-A3F6-4D85-AC52-48197421F140}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9523</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1593,36 +2647,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="10.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="9.06640625" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>44379</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2">
+        <v>3.2199999999999999E-2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2.3300000000000001E-2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>5.4699999999999999E-2</v>
+      </c>
+      <c r="F2" s="2">
+        <f>MIN(D2 - 0.02,E2)</f>
+        <v>3.3000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>44411</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.4799999999999999E-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.7500000000000002E-2</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" ref="F3:F9" si="0">MIN(D3 - 0.02,E3)</f>
+        <v>-3.599999999999999E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>44455</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.4200000000000001E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3.0099999999999998E-2</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.3999999999999994E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>44484</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2">
+        <v>3.6900000000000002E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.44E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="0"/>
+        <v>-5.6000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>44501</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2">
+        <v>2.6200000000000001E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.78E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.11E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>-2.2000000000000006E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>44551</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2.6499999999999999E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="0"/>
+        <v>-8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>44586</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>44607</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3.3099999999999997E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>1.89E-2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="0"/>
+        <v>-1.1000000000000003E-3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1630,11 +2858,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F2CCC9-7810-43B3-B79E-716FDC852CE6}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S23" sqref="S23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -1644,16 +2875,16 @@
       <c r="B1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1664,18 +2895,18 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>1.76</v>
-      </c>
-      <c r="D2">
-        <v>1.07</v>
-      </c>
-      <c r="E2">
-        <v>1.44</v>
-      </c>
-      <c r="F2">
+      <c r="C2" s="2">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1.44E-2</v>
+      </c>
+      <c r="F2" s="2">
         <f>MIN(D2 - 0.02,E2)</f>
-        <v>1.05</v>
+        <v>-9.300000000000001E-3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
@@ -1685,18 +2916,18 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>1.39</v>
-      </c>
-      <c r="E3">
-        <v>1.23</v>
-      </c>
-      <c r="F3">
+      <c r="C3" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1.23E-2</v>
+      </c>
+      <c r="F3" s="2">
         <f t="shared" ref="F3:F9" si="0">MIN(D3 - 0.02,E3)</f>
-        <v>1.23</v>
+        <v>-6.1000000000000013E-3</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -1706,18 +2937,18 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4">
-        <v>1.6</v>
-      </c>
-      <c r="D4">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="E4">
-        <v>0.93</v>
-      </c>
-      <c r="F4">
+      <c r="C4" s="2">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1.15E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>0.93</v>
+        <v>-8.5000000000000006E-3</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
@@ -1727,18 +2958,18 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5">
-        <v>1.65</v>
-      </c>
-      <c r="D5">
-        <v>1.08</v>
-      </c>
-      <c r="E5">
-        <v>1.19</v>
-      </c>
-      <c r="F5">
+      <c r="C5" s="2">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>1.06</v>
+        <v>-9.1999999999999998E-3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
@@ -1748,18 +2979,18 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6">
-        <v>2.04</v>
-      </c>
-      <c r="D6">
-        <v>1.47</v>
-      </c>
-      <c r="E6">
-        <v>1.42</v>
-      </c>
-      <c r="F6">
+      <c r="C6" s="2">
+        <v>2.0400000000000001E-2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>1.47E-2</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>1.42</v>
+        <v>-5.3000000000000009E-3</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
@@ -1769,18 +3000,18 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7">
-        <v>1.83</v>
-      </c>
-      <c r="D7">
-        <v>1.43</v>
-      </c>
-      <c r="E7">
-        <v>1.21</v>
-      </c>
-      <c r="F7">
+      <c r="C7" s="2">
+        <v>1.83E-2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1.43E-2</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1.21E-2</v>
+      </c>
+      <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>1.21</v>
+        <v>-5.7000000000000002E-3</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
@@ -1790,18 +3021,18 @@
       <c r="B8" t="s">
         <v>8</v>
       </c>
-      <c r="C8">
-        <v>1.79</v>
-      </c>
-      <c r="D8">
-        <v>1.32</v>
-      </c>
-      <c r="E8">
-        <v>1.03</v>
-      </c>
-      <c r="F8">
+      <c r="C8" s="2">
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1.32E-2</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1.03E-2</v>
+      </c>
+      <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>1.03</v>
+        <v>-6.8000000000000005E-3</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
@@ -1811,22 +3042,23 @@
       <c r="B9" t="s">
         <v>14</v>
       </c>
-      <c r="C9">
-        <v>1.49</v>
-      </c>
-      <c r="D9">
-        <v>0.78</v>
-      </c>
-      <c r="E9">
-        <v>1.07</v>
-      </c>
-      <c r="F9">
+      <c r="C9" s="2">
+        <v>1.49E-2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="E9" s="2">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>0.76</v>
+        <v>-1.2200000000000001E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
April 14, 2022, 方舟/号角
</commit_message>
<xml_diff>
--- a/历史出率.xlsx
+++ b/历史出率.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\Vtuber\Tools\GachaStatistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCA1AA2-5C35-4A8E-9616-FCE471A7CE18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55DDE84-522E-463D-87B3-EADDD21E9EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="16080" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>日期</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>菲亚梅塔</t>
+  </si>
+  <si>
+    <t>号角</t>
   </si>
 </sst>
 </file>
@@ -284,9 +287,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>方舟!$B$2:$B$10</c:f>
+              <c:f>方舟!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>帕拉斯</c:v>
                 </c:pt>
@@ -313,16 +316,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>菲亚梅塔</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>号角</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>方舟!$C$2:$C$10</c:f>
+              <c:f>方舟!$C$2:$C$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>3.2199999999999999E-2</c:v>
                 </c:pt>
@@ -349,6 +355,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2.6700000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.15E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -401,9 +410,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>方舟!$B$2:$B$10</c:f>
+              <c:f>方舟!$B$2:$B$11</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>帕拉斯</c:v>
                 </c:pt>
@@ -430,16 +439,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>菲亚梅塔</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>号角</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>方舟!$D$2:$D$10</c:f>
+              <c:f>方舟!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>2.3300000000000001E-2</c:v>
                 </c:pt>
@@ -466,6 +478,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1.2800000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.26E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2662,10 +2677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2732,7 +2747,7 @@
         <v>1.7500000000000002E-2</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F10" si="0">MIN(D3 - 0.02,E3)</f>
+        <f t="shared" ref="F3:F11" si="0">MIN(D3 - 0.02,E3)</f>
         <v>-3.599999999999999E-3</v>
       </c>
     </row>
@@ -2881,6 +2896,27 @@
       <c r="F10" s="2">
         <f t="shared" si="0"/>
         <v>-7.1999999999999998E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A11" s="1">
+        <v>44665</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2">
+        <v>3.15E-2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>1.26E-2</v>
+      </c>
+      <c r="E11" s="2">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="0"/>
+        <v>-7.4000000000000003E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>